<commit_message>
Updated supplementary table 3
</commit_message>
<xml_diff>
--- a/results/supplementary/FEEspinosadelAlbaST3.xlsx
+++ b/results/supplementary/FEEspinosadelAlbaST3.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -143,6 +143,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -150,9 +153,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,37 +494,37 @@
       <selection activeCell="A12" sqref="A12:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.046875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="68.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.640625" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.91015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.18359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.9765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
@@ -540,8 +540,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -560,8 +560,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -578,8 +578,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -596,17 +596,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
@@ -622,8 +622,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -642,8 +642,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="7"/>
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
@@ -660,8 +660,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -678,15 +678,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="1"/>
     </row>
   </sheetData>

</xml_diff>